<commit_message>
update planning and adding .side
</commit_message>
<xml_diff>
--- a/tareas/planning/Planning.xlsx
+++ b/tareas/planning/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eve_3\repo\intro_automation\tareas\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AD136F-C1F1-4B30-AFF5-4F91BAFE440C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9926DC0B-9404-4FE4-97E7-96911A342B93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="585" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>